<commit_message>
trying to make the writing to excel file a little cleaner. removed some junk code.
</commit_message>
<xml_diff>
--- a/osrsItems.xlsx
+++ b/osrsItems.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="19">
   <si>
     <t>Item</t>
   </si>
@@ -28,55 +28,49 @@
     <t>Sell Price</t>
   </si>
   <si>
-    <t>Margin</t>
-  </si>
-  <si>
     <t>zulrah-s-scales</t>
   </si>
   <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>221</t>
+    <t>237</t>
+  </si>
+  <si>
+    <t>236</t>
   </si>
   <si>
     <t>blood-rune</t>
   </si>
   <si>
-    <t>326</t>
-  </si>
-  <si>
-    <t>325</t>
-  </si>
-  <si>
-    <t>327</t>
+    <t>323</t>
+  </si>
+  <si>
+    <t>324</t>
   </si>
   <si>
     <t>grimy-toadflax</t>
   </si>
   <si>
-    <t>1,937</t>
-  </si>
-  <si>
-    <t>1,989</t>
+    <t>2,051</t>
+  </si>
+  <si>
+    <t>2,050</t>
+  </si>
+  <si>
+    <t>2,053</t>
   </si>
   <si>
     <t>mist-rune</t>
   </si>
   <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>88</t>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
   </si>
   <si>
     <t>revenant-ether</t>
   </si>
   <si>
-    <t>176</t>
+    <t>174</t>
   </si>
 </sst>
 </file>
@@ -408,13 +402,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,13 +421,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -445,23 +436,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -473,32 +464,32 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>